<commit_message>
Disable lastvisit constraint for testing
</commit_message>
<xml_diff>
--- a/app/config/tables/MIF_VISIT/forms/MIF_VISIT/MIF_VISIT.xlsx
+++ b/app/config/tables/MIF_VISIT/forms/MIF_VISIT/MIF_VISIT.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D648E730-88F0-406D-A8F4-D772A18FF4B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6C4312-8B4C-45F4-B487-D9C31DA77039}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="319">
   <si>
     <t>setting_name</t>
   </si>
@@ -1603,11 +1603,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:K102"/>
+  <dimension ref="A1:L102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,7 +1625,7 @@
     <col min="11" max="11" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>137</v>
       </c>
@@ -1659,14 +1659,17 @@
       <c r="K1" s="27" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>265</v>
       </c>
@@ -1680,7 +1683,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>133</v>
       </c>
@@ -1697,17 +1700,17 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>133</v>
       </c>
@@ -1724,7 +1727,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>134</v>
       </c>
@@ -1732,7 +1735,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>265</v>
       </c>
@@ -1746,7 +1749,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>133</v>
       </c>
@@ -1763,7 +1766,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>134</v>
       </c>
@@ -1771,7 +1774,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>131</v>
       </c>
@@ -1785,23 +1788,23 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
       <c r="B16" t="s">
         <v>134</v>
@@ -1974,7 +1977,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>269</v>
       </c>
@@ -1985,17 +1988,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>134</v>
       </c>
@@ -2003,20 +2006,23 @@
         <v>187</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>134</v>
       </c>
       <c r="C37" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L38" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>133</v>
       </c>
@@ -2039,17 +2045,17 @@
         <v>273</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>134</v>
       </c>
@@ -2057,12 +2063,12 @@
         <v>165</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>265</v>
       </c>
@@ -2076,7 +2082,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>133</v>
       </c>
@@ -2093,7 +2099,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>133</v>
       </c>
@@ -2110,12 +2116,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>134</v>
       </c>

</xml_diff>